<commit_message>
Adding upadted xlsx file
</commit_message>
<xml_diff>
--- a/Orders_restaurants_analysis.xlsx
+++ b/Orders_restaurants_analysis.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpatl\Desktop\Github projects\Restaurant-data-analysis-in-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27098439-26E6-4DBF-BEA4-B3C59E501A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5C7B58-6A04-44C6-82BF-4C288D2C67C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
     <pivotCache cacheId="2" r:id="rId6"/>
     <pivotCache cacheId="3" r:id="rId7"/>
     <pivotCache cacheId="4" r:id="rId8"/>
-    <pivotCache cacheId="5" r:id="rId9"/>
+    <pivotCache cacheId="17" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1846,9 +1846,6 @@
     <t>Average of Customer Rating-Delivery</t>
   </si>
   <si>
-    <t>What is the average customers rating points for food and delivery?</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -1910,6 +1907,9 @@
   </si>
   <si>
     <t>What is the most used mode of payment by customers?</t>
+  </si>
+  <si>
+    <t>What is the Average customer ratings for food and delivery services?</t>
   </si>
 </sst>
 </file>
@@ -1968,7 +1968,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1983,19 +1983,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="40">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-14009]hh:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="165" formatCode="[$-14009]hh:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-14009]hh:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-14009]hh:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2026,6 +2056,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -10340,16 +10379,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>117</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11116,24 +11155,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Mitali Patle" refreshedDate="44940.031898379631" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{4A7DDC8E-D753-47E5-8C1A-628403B4F713}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Mitali Patle" refreshedDate="44955.480307638885" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{4A7DDC8E-D753-47E5-8C1A-628403B4F713}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
     <cacheField name="[Measures].[Count of Order ID]" caption="Count of Order ID" numFmtId="0" hierarchy="28" level="32767"/>
     <cacheField name="[Table2].[O Time].[O Time]" caption="O Time" numFmtId="0" hierarchy="7" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T11:10:00" maxDate="1899-12-30T11:19:00" count="4">
-        <d v="1899-12-30T11:10:00"/>
-        <d v="1899-12-30T11:15:00"/>
-        <d v="1899-12-30T11:17:00"/>
-        <d v="1899-12-30T11:19:00"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T22:01:00" maxDate="1899-12-30T22:01:00" count="1">
+        <d v="1899-12-30T22:01:00"/>
       </sharedItems>
       <extLst>
         <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{4F2E5C28-24EA-4eb8-9CBF-B6C8F9C3D259}">
           <x15:cachedUniqueNames>
-            <x15:cachedUniqueName index="0" name="[Table2].[O Time].&amp;[1899-12-30T11:10:00]"/>
-            <x15:cachedUniqueName index="1" name="[Table2].[O Time].&amp;[1899-12-30T11:15:00]"/>
-            <x15:cachedUniqueName index="2" name="[Table2].[O Time].&amp;[1899-12-30T11:17:00]"/>
-            <x15:cachedUniqueName index="3" name="[Table2].[O Time].&amp;[1899-12-30T11:19:00]"/>
+            <x15:cachedUniqueName index="0" name="[Table2].[O Time].&amp;[1899-12-30T22:01:00]"/>
           </x15:cachedUniqueNames>
         </ext>
       </extLst>
@@ -11273,457 +11306,17 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{810C5043-7BE6-440E-8464-C7E1988B76C8}" name="PivotTable12" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Restaurants">
-  <location ref="A5:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="20">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="21">
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Total sales after discount" fld="1" baseField="0" baseItem="16" numFmtId="2"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="1">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotHierarchies count="29">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1" caption="Total sales after discount"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-  </pivotHierarchies>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="3"/>
-  </rowHierarchiesUsage>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Orders.xlsx!Table2">
-        <x15:activeTabTopLevelEntity name="[Table2]"/>
-      </x15:pivotTableUISettings>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{010D31FF-BECD-421A-943F-2D52227780C8}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Restaurants">
-  <location ref="A94:C115" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="20">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="21">
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Average of Customer Rating-Food" fld="0" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
-    <dataField name="Average of Customer Rating-Delivery" fld="2" subtotal="average" baseField="1" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="2">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="7">
-    <chartFormat chart="4" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="6" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="6" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="6" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="18"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotHierarchies count="29">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1" caption="Average of Delivery Time Taken (mins)"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1" caption="Average of Customer Rating-Food"/>
-    <pivotHierarchy dragToData="1" caption="Average of Customer Rating-Delivery"/>
-    <pivotHierarchy dragToData="1"/>
-  </pivotHierarchies>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="3"/>
-  </rowHierarchiesUsage>
-  <colHierarchiesUsage count="1">
-    <colHierarchyUsage hierarchyUsage="-2"/>
-  </colHierarchiesUsage>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Orders.xlsx!Table2">
-        <x15:activeTabTopLevelEntity name="[Table2]"/>
-      </x15:pivotTableUISettings>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ECE7C0BE-21D8-41B9-B6C1-D603C02FC2D1}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14" rowHeaderCaption="Time(hours)">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ECE7C0BE-21D8-41B9-B6C1-D603C02FC2D1}" name="PivotTable3" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14" rowHeaderCaption="Time(hours)">
   <location ref="A122:B135" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
-      <items count="5">
+      <items count="2">
         <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" defaultSubtotal="0">
       <items count="12">
         <item x="0" e="0"/>
         <item x="1" e="0"/>
@@ -11792,17 +11385,17 @@
     <dataField name="Number of orders" fld="0" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="5">
+    <format dxfId="14">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
@@ -11873,7 +11466,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EFDD6387-F1DD-42F4-A545-49705C464171}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Mode of payment">
   <location ref="A76:B80" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
@@ -11940,7 +11533,7 @@
     <dataField name="% of customers " fld="1" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="1" numFmtId="9"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="7">
+    <format dxfId="16">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -11949,7 +11542,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="15">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -12060,7 +11653,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BD0683F6-6176-430A-A24C-0015E0C4B80B}" name="PivotTable14" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Cuisine">
   <location ref="A57:B66" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
@@ -12126,7 +11719,7 @@
     <dataField name="% popularity of cuisine " fld="1" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="1" numFmtId="9"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="10">
+    <format dxfId="19">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -12135,14 +11728,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="18">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="17">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -12304,7 +11897,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{389CAC28-1DC0-4C4E-A25B-ACA4D2826B60}" name="PivotTable13" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Restaurants">
   <location ref="A31:B52" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
@@ -12418,14 +12011,14 @@
     <dataField name="Average of Delivery Time Taken (mins)" fld="1" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="12">
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="20">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -12491,38 +12084,475 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{810C5043-7BE6-440E-8464-C7E1988B76C8}" name="PivotTable12" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Restaurants">
+  <location ref="A5:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="20">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="21">
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Total sales after discount" fld="1" baseField="0" baseItem="16" numFmtId="2"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="23">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotHierarchies count="29">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1" caption="Total sales after discount"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="3"/>
+  </rowHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Orders.xlsx!Table2">
+        <x15:activeTabTopLevelEntity name="[Table2]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{010D31FF-BECD-421A-943F-2D52227780C8}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Restaurants">
+  <location ref="A94:C115" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="20">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="21">
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Average of Customer Rating-Food" fld="0" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
+    <dataField name="Average of Customer Rating-Delivery" fld="2" subtotal="average" baseField="1" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="24">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="7">
+    <chartFormat chart="4" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotHierarchies count="29">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1" caption="Average of Delivery Time Taken (mins)"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1" caption="Average of Customer Rating-Food"/>
+    <pivotHierarchy dragToData="1" caption="Average of Customer Rating-Delivery"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="3"/>
+  </rowHierarchiesUsage>
+  <colHierarchiesUsage count="1">
+    <colHierarchyUsage hierarchyUsage="-2"/>
+  </colHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Orders.xlsx!Table2">
+        <x15:activeTabTopLevelEntity name="[Table2]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F37FE743-B536-42B4-A350-6E3AEEB32296}" name="Table2" displayName="Table2" ref="A1:P501" totalsRowShown="0">
   <autoFilter ref="A1:P501" xr:uid="{F37FE743-B536-42B4-A350-6E3AEEB32296}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{E6B5BB71-086A-49CD-99B0-5FAD912AEAD7}" name="Order ID"/>
-    <tableColumn id="2" xr3:uid="{44B1F368-43D2-425F-8A78-4192319B574B}" name="Customer Name" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{AD3510C6-154F-4D6B-B73C-06B69AFC5A80}" name="Restaurant ID" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{0EA227B4-F2C5-4A3A-9186-0C45A77018B0}" name="Restaurant Name" dataDxfId="25">
+    <tableColumn id="2" xr3:uid="{44B1F368-43D2-425F-8A78-4192319B574B}" name="Customer Name" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{AD3510C6-154F-4D6B-B73C-06B69AFC5A80}" name="Restaurant ID" dataDxfId="38"/>
+    <tableColumn id="13" xr3:uid="{0EA227B4-F2C5-4A3A-9186-0C45A77018B0}" name="Restaurant Name" dataDxfId="37">
       <calculatedColumnFormula>VLOOKUP(C2,'Restaurant Details'!$A$1:$E$21,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{EA557884-24E2-4E07-92E0-575B6581D213}" name="Cuisine" dataDxfId="24">
+    <tableColumn id="14" xr3:uid="{EA557884-24E2-4E07-92E0-575B6581D213}" name="Cuisine" dataDxfId="36">
       <calculatedColumnFormula>VLOOKUP(C2,'Restaurant Details'!$A$2:$C$21,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1820EE62-280F-46E1-A7EB-9C9E12B1DDAB}" name="Order Date" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{74A5B552-AB38-4D40-ADE5-97EC7EC79DA2}" name="O Date" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{1820EE62-280F-46E1-A7EB-9C9E12B1DDAB}" name="Order Date" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{74A5B552-AB38-4D40-ADE5-97EC7EC79DA2}" name="O Date" dataDxfId="34">
       <calculatedColumnFormula>INT(F2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0976BC8E-54CE-4024-B818-BD2EF373B64C}" name="O Time" dataDxfId="21">
+    <tableColumn id="12" xr3:uid="{0976BC8E-54CE-4024-B818-BD2EF373B64C}" name="O Time" dataDxfId="33">
       <calculatedColumnFormula>F2-INT(F2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FB13C816-C353-4AFD-8BD1-AEFA0C2B745C}" name="Quantity of Items" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{FE8B2ABA-361E-48C4-A977-5B8B98A6DB9A}" name="Order Amount" dataDxfId="19"/>
-    <tableColumn id="15" xr3:uid="{A19ABC49-4E9E-4DE2-AF68-1EA3CAD68322}" name="Discount " dataDxfId="18">
+    <tableColumn id="5" xr3:uid="{FB13C816-C353-4AFD-8BD1-AEFA0C2B745C}" name="Quantity of Items" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{FE8B2ABA-361E-48C4-A977-5B8B98A6DB9A}" name="Order Amount" dataDxfId="31"/>
+    <tableColumn id="15" xr3:uid="{A19ABC49-4E9E-4DE2-AF68-1EA3CAD68322}" name="Discount " dataDxfId="30">
       <calculatedColumnFormula>IF(J2&gt;=500,"Y","N")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{1A00F1D0-018F-4AC2-BF61-6E0712353F11}" name="Discounted Amount" dataDxfId="17">
+    <tableColumn id="16" xr3:uid="{1A00F1D0-018F-4AC2-BF61-6E0712353F11}" name="Discounted Amount" dataDxfId="29">
       <calculatedColumnFormula>IF(J2&gt;=500,0.95*J2,J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9EFE0079-1F02-49EB-BFE6-144DA73BB93B}" name="Payment Mode" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{FB97CA47-622D-4E2C-9FB9-E1BE3C88B9D2}" name="Delivery Time Taken (mins)" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{439A6E9D-5BEE-40DA-B4AE-B6464F0CAC2F}" name="Customer Rating-Food" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{57823024-65C5-4073-ACC0-272596A66C48}" name="Customer Rating-Delivery" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{9EFE0079-1F02-49EB-BFE6-144DA73BB93B}" name="Payment Mode" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{FB97CA47-622D-4E2C-9FB9-E1BE3C88B9D2}" name="Delivery Time Taken (mins)" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{439A6E9D-5BEE-40DA-B4AE-B6464F0CAC2F}" name="Customer Rating-Food" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{57823024-65C5-4073-ACC0-272596A66C48}" name="Customer Rating-Delivery" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -41255,8 +41285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1CCCEC7-316B-472D-9C25-22AB2D349A4A}">
   <dimension ref="A4:I135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41365,10 +41395,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B5" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -41546,7 +41576,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B31" t="s">
         <v>577</v>
@@ -41730,7 +41760,7 @@
         <v>570</v>
       </c>
       <c r="B57" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -41810,15 +41840,15 @@
     </row>
     <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B76" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -41855,12 +41885,12 @@
     </row>
     <row r="93" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A93" s="11" t="s">
-        <v>585</v>
+        <v>606</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B94" t="s">
         <v>583</v>
@@ -42102,108 +42132,108 @@
     </row>
     <row r="120" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A120" s="11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B122" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="7" t="s">
-        <v>586</v>
+      <c r="A123" s="12" t="s">
+        <v>585</v>
       </c>
       <c r="B123" s="3">
         <v>73</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" s="7" t="s">
-        <v>587</v>
+      <c r="A124" s="12" t="s">
+        <v>586</v>
       </c>
       <c r="B124" s="3">
         <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="7" t="s">
-        <v>588</v>
+      <c r="A125" s="12" t="s">
+        <v>587</v>
       </c>
       <c r="B125" s="3">
         <v>54</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="7" t="s">
-        <v>589</v>
+      <c r="A126" s="12" t="s">
+        <v>588</v>
       </c>
       <c r="B126" s="3">
         <v>99</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" s="7" t="s">
-        <v>590</v>
+      <c r="A127" s="12" t="s">
+        <v>589</v>
       </c>
       <c r="B127" s="3">
         <v>23</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="7" t="s">
-        <v>591</v>
+      <c r="A128" s="12" t="s">
+        <v>590</v>
       </c>
       <c r="B128" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="7" t="s">
-        <v>592</v>
+      <c r="A129" s="12" t="s">
+        <v>591</v>
       </c>
       <c r="B129" s="3">
         <v>18</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="7" t="s">
-        <v>593</v>
+      <c r="A130" s="12" t="s">
+        <v>592</v>
       </c>
       <c r="B130" s="3">
         <v>31</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="7" t="s">
-        <v>594</v>
+      <c r="A131" s="12" t="s">
+        <v>593</v>
       </c>
       <c r="B131" s="3">
         <v>49</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="7" t="s">
-        <v>595</v>
+      <c r="A132" s="12" t="s">
+        <v>594</v>
       </c>
       <c r="B132" s="3">
         <v>31</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="7" t="s">
-        <v>596</v>
+      <c r="A133" s="12" t="s">
+        <v>595</v>
       </c>
       <c r="B133" s="3">
         <v>15</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="7" t="s">
-        <v>597</v>
+      <c r="A134" s="12" t="s">
+        <v>596</v>
       </c>
       <c r="B134" s="3">
         <v>46</v>

</xml_diff>